<commit_message>
Added total volume of brew water for ease of use in some workflows
</commit_message>
<xml_diff>
--- a/20230108 - 4-6 Pour Over Spready.xlsx
+++ b/20230108 - 4-6 Pour Over Spready.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://coreygallon-my.sharepoint.com/personal/corey_gallon_me/Documents/Documents/coffee/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="148" documentId="8_{D8CD47BF-5BDE-4379-8F3A-E78FF9B3C88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90C4B44B-1F59-480A-905B-547095F90C92}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="8_{D8CD47BF-5BDE-4379-8F3A-E78FF9B3C88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42D3FB0D-E080-403E-8D30-2982BC1FC5DC}"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="735" windowWidth="21630" windowHeight="14145" xr2:uid="{45B253CB-A6BD-44EA-8F9A-CF5F0FE0DFC6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{45B253CB-A6BD-44EA-8F9A-CF5F0FE0DFC6}"/>
   </bookViews>
   <sheets>
     <sheet name="4-6 Pour Over Recipe" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Dose Required (g)</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>https://youtu.be/wmCW8xSWGZY</t>
+  </si>
+  <si>
+    <t>Total (g)</t>
   </si>
 </sst>
 </file>
@@ -300,7 +303,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -375,10 +378,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -670,7 +669,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -679,9 +678,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F2DA34-4714-4969-8F04-D054DCAE30C2}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:J19"/>
+  <dimension ref="B2:K19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -690,7 +691,7 @@
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="20" t="s">
         <v>10</v>
       </c>
@@ -698,7 +699,7 @@
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
@@ -706,70 +707,70 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="19">
         <f>ROUNDUP(target_brew_mass/(brew_ratio-2),0)</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C7">
         <f>C6*C5</f>
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="E8" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C9">
         <f>dose * 2</f>
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="14">
         <f>0.4*(water-bloom)</f>
-        <v>161.20000000000002</v>
+        <v>162</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="15">
         <f>0.6*(water-bloom)</f>
-        <v>241.79999999999998</v>
+        <v>243</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>21</v>
@@ -779,10 +780,10 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="8" t="s">
         <v>4</v>
@@ -791,14 +792,17 @@
         <v>8</v>
       </c>
       <c r="E13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
@@ -807,15 +811,19 @@
       </c>
       <c r="D14" s="16">
         <f>bloom</f>
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E14" s="19">
+        <f>D14</f>
+        <v>54</v>
+      </c>
+      <c r="F14" s="19">
         <f>water-bloom</f>
-        <v>403</v>
-      </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
@@ -825,15 +833,19 @@
       </c>
       <c r="D15" s="17">
         <f>C15*forty</f>
-        <v>53.733333333333334</v>
+        <v>54</v>
       </c>
       <c r="E15" s="14">
-        <f>E14-first_pour</f>
-        <v>349.26666666666665</v>
-      </c>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+        <f>E14+D15</f>
+        <v>108</v>
+      </c>
+      <c r="F15" s="14">
+        <f>F14-first_pour</f>
+        <v>351</v>
+      </c>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
@@ -843,15 +855,19 @@
       </c>
       <c r="D16" s="17">
         <f>C16*forty</f>
-        <v>107.46666666666667</v>
+        <v>108</v>
       </c>
       <c r="E16" s="14">
-        <f>E15-second_pour</f>
-        <v>241.79999999999998</v>
-      </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E16:E19" si="0">E15+D16</f>
+        <v>216</v>
+      </c>
+      <c r="F16" s="14">
+        <f>F15-second_pour</f>
+        <v>243</v>
+      </c>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
@@ -861,15 +877,19 @@
       </c>
       <c r="D17" s="18">
         <f>C17*sixty</f>
-        <v>161.19999999999999</v>
+        <v>162</v>
       </c>
       <c r="E17" s="15">
-        <f>E16-third_pour</f>
-        <v>80.599999999999994</v>
-      </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>378</v>
+      </c>
+      <c r="F17" s="15">
+        <f>F16-third_pour</f>
+        <v>81</v>
+      </c>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
@@ -879,15 +899,19 @@
       </c>
       <c r="D18" s="18">
         <f>C18*sixty</f>
-        <v>80.599999999999994</v>
+        <v>81</v>
       </c>
       <c r="E18" s="15">
-        <f>E17-fourth_pour</f>
+        <f t="shared" si="0"/>
+        <v>459</v>
+      </c>
+      <c r="F18" s="15">
+        <f>F17-fourth_pour</f>
         <v>0</v>
       </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>15</v>
       </c>
@@ -899,16 +923,20 @@
         <v>0</v>
       </c>
       <c r="E19" s="15">
-        <f>E18-fifth_pour</f>
+        <f t="shared" si="0"/>
+        <v>459</v>
+      </c>
+      <c r="F19" s="15">
+        <f>F18-fifth_pour</f>
         <v>0</v>
       </c>
-      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="40% of Water Configuration Error" error="% of water poured in 1st and 2nd pours must sum to 100%" sqref="C15:C16" xr:uid="{A785EF84-131E-4F08-B5F2-F27882453BDC}">
       <formula1>SUM(C15:C16)=1</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Removed data validation & updated latest recipe
</commit_message>
<xml_diff>
--- a/20230108 - 4-6 Pour Over Spready.xlsx
+++ b/20230108 - 4-6 Pour Over Spready.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://coreygallon-my.sharepoint.com/personal/corey_gallon_me/Documents/Documents/coffee/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="186" documentId="8_{D8CD47BF-5BDE-4379-8F3A-E78FF9B3C88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42D3FB0D-E080-403E-8D30-2982BC1FC5DC}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="8_{D8CD47BF-5BDE-4379-8F3A-E78FF9B3C88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD5ECC60-500A-4015-836B-D71724B83F95}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{45B253CB-A6BD-44EA-8F9A-CF5F0FE0DFC6}"/>
+    <workbookView xWindow="4245" yWindow="1425" windowWidth="21630" windowHeight="14145" xr2:uid="{45B253CB-A6BD-44EA-8F9A-CF5F0FE0DFC6}"/>
   </bookViews>
   <sheets>
     <sheet name="4-6 Pour Over Recipe" sheetId="1" r:id="rId1"/>
@@ -305,20 +305,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>515408</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:rowOff>10584</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:colOff>31750</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>172508</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
+        <xdr:cNvPr id="3" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{079E60A7-2A95-909F-053F-349C50A6CD07}"/>
@@ -378,6 +378,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -669,7 +673,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -681,7 +685,7 @@
   <dimension ref="B2:K19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +862,7 @@
         <v>108</v>
       </c>
       <c r="E16" s="14">
-        <f t="shared" ref="E16:E19" si="0">E15+D16</f>
+        <f>E15+D16</f>
         <v>216</v>
       </c>
       <c r="F16" s="14">
@@ -872,20 +876,19 @@
         <v>13</v>
       </c>
       <c r="C17" s="10">
-        <f>2/3</f>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="D17" s="18">
         <f>C17*sixty</f>
-        <v>162</v>
+        <v>121.5</v>
       </c>
       <c r="E17" s="15">
-        <f t="shared" si="0"/>
-        <v>378</v>
+        <f>E16+D17</f>
+        <v>337.5</v>
       </c>
       <c r="F17" s="15">
         <f>F16-third_pour</f>
-        <v>81</v>
+        <v>121.5</v>
       </c>
       <c r="H17" s="2"/>
     </row>
@@ -894,15 +897,14 @@
         <v>14</v>
       </c>
       <c r="C18" s="10">
-        <f>1/3</f>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
       <c r="D18" s="18">
         <f>C18*sixty</f>
-        <v>81</v>
+        <v>121.5</v>
       </c>
       <c r="E18" s="15">
-        <f t="shared" si="0"/>
+        <f>E17+D18</f>
         <v>459</v>
       </c>
       <c r="F18" s="15">
@@ -915,15 +917,13 @@
       <c r="B19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="10">
-        <v>0</v>
-      </c>
+      <c r="C19" s="10"/>
       <c r="D19" s="18">
         <f>C19*sixty</f>
         <v>0</v>
       </c>
       <c r="E19" s="15">
-        <f t="shared" si="0"/>
+        <f>E18+D19</f>
         <v>459</v>
       </c>
       <c r="F19" s="15">
@@ -936,12 +936,9 @@
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="40% of Water Configuration Error" error="% of water poured in 1st and 2nd pours must sum to 100%" sqref="C15:C16" xr:uid="{A785EF84-131E-4F08-B5F2-F27882453BDC}">
       <formula1>SUM(C15:C16)=1</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="60% of Water Configuration Error" error="% of water poured in 3rd, 4th and 5th pours must sum to 100%" sqref="C17:C19" xr:uid="{E59C4768-7482-419F-A821-C8471C43A7F2}">
-      <formula1>SUM(C17:C19)=1</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>

<commit_message>
added charts for pour over
</commit_message>
<xml_diff>
--- a/20230108 - 4-6 Pour Over Spready.xlsx
+++ b/20230108 - 4-6 Pour Over Spready.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://coreygallon-my.sharepoint.com/personal/corey_gallon_me/Documents/Documents/coffee/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="209" documentId="8_{D8CD47BF-5BDE-4379-8F3A-E78FF9B3C88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD5ECC60-500A-4015-836B-D71724B83F95}"/>
+  <xr:revisionPtr revIDLastSave="246" documentId="8_{D8CD47BF-5BDE-4379-8F3A-E78FF9B3C88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{229F6D1D-5BA4-42B3-A256-61BF2728C765}"/>
   <bookViews>
-    <workbookView xWindow="4245" yWindow="1425" windowWidth="21630" windowHeight="14145" xr2:uid="{45B253CB-A6BD-44EA-8F9A-CF5F0FE0DFC6}"/>
+    <workbookView xWindow="29430" yWindow="2325" windowWidth="18255" windowHeight="18660" xr2:uid="{45B253CB-A6BD-44EA-8F9A-CF5F0FE0DFC6}"/>
   </bookViews>
   <sheets>
     <sheet name="4-6 Pour Over Recipe" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +203,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -254,20 +278,18 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -277,11 +299,26 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -299,6 +336,1843 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>The Pours</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (mL)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'4-6 Pour Over Recipe'!$B$15:$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1st Pour (Acidity)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2nd Pour (Sweetness)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3rd Pour (Strength)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4th Pour (Strength)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5th Pour (Strength)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'4-6 Pour Over Recipe'!$D$15:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F04E-4838-9325-D3BAD46EB23C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="1086944944"/>
+        <c:axId val="1086949264"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1086944944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1086949264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1086949264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1086944944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Composition</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'4-6 Pour Over Recipe'!$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1st Pour (Acidity)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'4-6 Pour Over Recipe'!$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>108</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8478-48D1-9471-B3F2CC7183C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'4-6 Pour Over Recipe'!$B$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2nd Pour (Sweetness)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'4-6 Pour Over Recipe'!$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>216</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8478-48D1-9471-B3F2CC7183C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'4-6 Pour Over Recipe'!$B$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3rd Pour (Strength)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'4-6 Pour Over Recipe'!$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>324</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8478-48D1-9471-B3F2CC7183C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'4-6 Pour Over Recipe'!$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4th Pour (Strength)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'4-6 Pour Over Recipe'!$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>243</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8478-48D1-9471-B3F2CC7183C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'4-6 Pour Over Recipe'!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5th Pour (Strength)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'4-6 Pour Over Recipe'!$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-8478-48D1-9471-B3F2CC7183C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="1656389712"/>
+        <c:axId val="1656405552"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1656389712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1656405552"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1656405552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1656389712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,17 +2251,85 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>509587</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>204787</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5D97D40-DEFE-CA5B-97A4-2C0E5BA9AB62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>452437</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D7F92A2-2DBB-3834-6558-DE9E248F2683}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -425,7 +2367,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -531,7 +2473,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -673,7 +2615,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -685,7 +2627,7 @@
   <dimension ref="B2:K19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,19 +2638,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="3">
-        <v>400</v>
+        <v>800</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -723,9 +2665,9 @@
       <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="16">
         <f>ROUNDUP(target_brew_mass/(brew_ratio-2),0)</f>
-        <v>27</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
@@ -734,15 +2676,15 @@
       </c>
       <c r="C7">
         <f>C6*C5</f>
-        <v>459</v>
-      </c>
-      <c r="E7" s="12" t="s">
+        <v>918</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="11" t="s">
         <v>19</v>
       </c>
     </row>
@@ -752,31 +2694,31 @@
       </c>
       <c r="C9">
         <f>dose * 2</f>
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="12">
         <f>0.4*(water-bloom)</f>
-        <v>162</v>
-      </c>
-      <c r="E10" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="13">
         <f>0.6*(water-bloom)</f>
-        <v>243</v>
-      </c>
-      <c r="E11" s="13" t="s">
+        <v>486</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>21</v>
       </c>
       <c r="G11" s="2"/>
@@ -789,16 +2731,16 @@
     </row>
     <row r="13" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="7" t="s">
         <v>9</v>
       </c>
       <c r="H13" s="2"/>
@@ -813,17 +2755,17 @@
       <c r="C14" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="14">
         <f>bloom</f>
-        <v>54</v>
-      </c>
-      <c r="E14" s="19">
+        <v>108</v>
+      </c>
+      <c r="E14" s="16">
         <f>D14</f>
-        <v>54</v>
-      </c>
-      <c r="F14" s="19">
+        <v>108</v>
+      </c>
+      <c r="F14" s="16">
         <f>water-bloom</f>
-        <v>405</v>
+        <v>810</v>
       </c>
       <c r="H14" s="2"/>
     </row>
@@ -831,104 +2773,105 @@
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="15">
         <f>C15*forty</f>
-        <v>54</v>
-      </c>
-      <c r="E15" s="14">
+        <v>108</v>
+      </c>
+      <c r="E15" s="12">
         <f>E14+D15</f>
-        <v>108</v>
-      </c>
-      <c r="F15" s="14">
+        <v>216</v>
+      </c>
+      <c r="F15" s="12">
         <f>F14-first_pour</f>
-        <v>351</v>
+        <v>702</v>
       </c>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="19">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="20">
         <f>C16*forty</f>
-        <v>108</v>
-      </c>
-      <c r="E16" s="14">
+        <v>216</v>
+      </c>
+      <c r="E16" s="21">
         <f>E15+D16</f>
-        <v>216</v>
-      </c>
-      <c r="F16" s="14">
+        <v>432</v>
+      </c>
+      <c r="F16" s="21">
         <f>F15-second_pour</f>
-        <v>243</v>
+        <v>486</v>
       </c>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="D17" s="18">
+      <c r="C17" s="23">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D17" s="24">
         <f>C17*sixty</f>
-        <v>121.5</v>
-      </c>
-      <c r="E17" s="15">
+        <v>324</v>
+      </c>
+      <c r="E17" s="25">
         <f>E16+D17</f>
-        <v>337.5</v>
-      </c>
-      <c r="F17" s="15">
+        <v>756</v>
+      </c>
+      <c r="F17" s="25">
         <f>F16-third_pour</f>
-        <v>121.5</v>
+        <v>162</v>
       </c>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="31">
         <v>0.5</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="32">
         <f>C18*sixty</f>
-        <v>121.5</v>
-      </c>
-      <c r="E18" s="15">
+        <v>243</v>
+      </c>
+      <c r="E18" s="33">
         <f>E17+D18</f>
-        <v>459</v>
-      </c>
-      <c r="F18" s="15">
+        <v>999</v>
+      </c>
+      <c r="F18" s="33">
         <f>F17-fourth_pour</f>
-        <v>0</v>
+        <v>-81</v>
       </c>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="18">
+      <c r="C19" s="27"/>
+      <c r="D19" s="28">
         <f>C19*sixty</f>
         <v>0</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="29">
         <f>E18+D19</f>
-        <v>459</v>
-      </c>
-      <c r="F19" s="15">
+        <v>999</v>
+      </c>
+      <c r="F19" s="29">
         <f>F18-fifth_pour</f>
-        <v>0</v>
+        <v>-81</v>
       </c>
       <c r="H19" s="2"/>
     </row>

</xml_diff>

<commit_message>
corrected stupid error in spready inputs
</commit_message>
<xml_diff>
--- a/20230108 - 4-6 Pour Over Spready.xlsx
+++ b/20230108 - 4-6 Pour Over Spready.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://coreygallon-my.sharepoint.com/personal/corey_gallon_me/Documents/Documents/coffee/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://coreygallon-my.sharepoint.com/personal/corey_gallon_me/Documents/Documents/coffee/pour_over/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="246" documentId="8_{D8CD47BF-5BDE-4379-8F3A-E78FF9B3C88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{229F6D1D-5BA4-42B3-A256-61BF2728C765}"/>
+  <xr:revisionPtr revIDLastSave="257" documentId="8_{D8CD47BF-5BDE-4379-8F3A-E78FF9B3C88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A551F028-6467-4AE3-A095-3B838A86E00D}"/>
   <bookViews>
-    <workbookView xWindow="29430" yWindow="2325" windowWidth="18255" windowHeight="18660" xr2:uid="{45B253CB-A6BD-44EA-8F9A-CF5F0FE0DFC6}"/>
+    <workbookView xWindow="8805" yWindow="1950" windowWidth="18255" windowHeight="18660" xr2:uid="{45B253CB-A6BD-44EA-8F9A-CF5F0FE0DFC6}"/>
   </bookViews>
   <sheets>
     <sheet name="4-6 Pour Over Recipe" sheetId="1" r:id="rId1"/>
@@ -300,9 +300,6 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -319,6 +316,9 @@
     <xf numFmtId="9" fontId="2" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -471,7 +471,7 @@
                   <c:v>324</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>243</c:v>
+                  <c:v>162.00000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -900,7 +900,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>243</c:v>
+                  <c:v>162.00000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2326,6 +2326,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -2627,7 +2631,7 @@
   <dimension ref="B2:K19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2638,12 +2642,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
@@ -2792,86 +2796,87 @@
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="18">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="19">
         <f>C16*forty</f>
         <v>216</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="20">
         <f>E15+D16</f>
         <v>432</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="20">
         <f>F15-second_pour</f>
         <v>486</v>
       </c>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="22">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="23">
         <f>C17*sixty</f>
         <v>324</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="24">
         <f>E16+D17</f>
         <v>756</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="24">
         <f>F16-third_pour</f>
         <v>162</v>
       </c>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="31">
-        <v>0.5</v>
-      </c>
-      <c r="D18" s="32">
+      <c r="C18" s="30">
+        <f>1-C17</f>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="D18" s="31">
         <f>C18*sixty</f>
-        <v>243</v>
-      </c>
-      <c r="E18" s="33">
+        <v>162.00000000000003</v>
+      </c>
+      <c r="E18" s="32">
         <f>E17+D18</f>
-        <v>999</v>
-      </c>
-      <c r="F18" s="33">
+        <v>918</v>
+      </c>
+      <c r="F18" s="32">
         <f>F17-fourth_pour</f>
-        <v>-81</v>
+        <v>0</v>
       </c>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="28">
+      <c r="C19" s="26"/>
+      <c r="D19" s="27">
         <f>C19*sixty</f>
         <v>0</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="28">
         <f>E18+D19</f>
-        <v>999</v>
-      </c>
-      <c r="F19" s="29">
+        <v>918</v>
+      </c>
+      <c r="F19" s="28">
         <f>F18-fifth_pour</f>
-        <v>-81</v>
+        <v>0</v>
       </c>
       <c r="H19" s="2"/>
     </row>

</xml_diff>